<commit_message>
Changed features once again.  trying to account for the same amount of attributes but in less features.  Using ratios as features.
</commit_message>
<xml_diff>
--- a/src/stats/docs/Model_Scores.xlsx
+++ b/src/stats/docs/Model_Scores.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13160" yWindow="7060" windowWidth="25600" windowHeight="18480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="52900" windowHeight="28320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -704,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1262,7 +1262,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>